<commit_message>
pending tasks: localstorage, year in admin charts, schedulings, acc statement validations, sp changings
</commit_message>
<xml_diff>
--- a/excel templates/profile-template.xlsx
+++ b/excel templates/profile-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhara\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhara\Desktop\MoneyFi\excel templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849BE587-3F16-48FE-8F27-3CB7B6952351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECADDEC-B598-4989-9109-6A57D9A4E676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A848DEA0-28D9-4EB4-9D65-99A50DB689DC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Phone Number</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,9 +442,39 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
+      <c r="A2">
+        <v>9381153612</v>
+      </c>
+      <c r="B2" s="2">
+        <v>37782</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>344</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{223DBEA3-1ED7-4C52-AEAF-B099139CE92C}">
+      <formula1>"Male,Femal,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{86B840A7-1DC5-4FA7-9998-0A08781DF231}">
+      <formula1>"Single,Married,Divorced,Widowed"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{8A4324B1-D26E-4895-8922-05ED9EB0C03A}">
+      <formula1>1</formula1>
+      <formula2>1E+46</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{8F99C1FD-105C-4A30-BEFB-1128D7414A6B}">
+      <formula1>AND(ISNUMBER(A2),LEN(A2)=10)</formula1>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{F2E81A6E-382A-441A-AA26-D5F3F2DEF7B4}">
+      <formula1>1</formula1>
+      <formula2>TODAY()</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>